<commit_message>
add test for PK Plots and sesnitivity
</commit_message>
<xml_diff>
--- a/inst/templates/Plots.xlsx
+++ b/inst/templates/Plots.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" state="visible" r:id="rId3"/>
@@ -16,8 +16,9 @@
     <sheet name="TimeRange" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="PKParameter_Boxplot" sheetId="7" state="visible" r:id="rId9"/>
     <sheet name="PKParameter_Forest" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="DemographicPlots" sheetId="9" state="visible" r:id="rId11"/>
-    <sheet name="SensitivityPlots" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="Histograms" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="DistributionVsRange" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="SensitivityPlots" sheetId="11" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="165">
   <si>
     <t xml:space="preserve">Scenario</t>
   </si>
@@ -457,12 +458,33 @@
     <t xml:space="preserve">xlimit used of log scale, should be something like c(0.1,NA) to set lower limit to 0.1</t>
   </si>
   <si>
+    <t xml:space="preserve">ParameterIds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario </t>
+  </si>
+  <si>
+    <t xml:space="preserve">used for comparsion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corresponds to name (identifier) of model or PK parameter, comma seperated list is split to plots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Needed only  if ParameterId is PKParameter, comma separated List is split to facets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scale of  x  axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limit used of linear scale, should be something like c(0,NA) to set lower limit to 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limit used of log scale, should be something like c(0.1,NA) to set lower limit to 0.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Scenarios</t>
   </si>
   <si>
-    <t xml:space="preserve">ParameterIds</t>
-  </si>
-  <si>
     <t xml:space="preserve">ParameterId_Bin</t>
   </si>
   <si>
@@ -472,43 +494,19 @@
     <t xml:space="preserve">NumberOfBins</t>
   </si>
   <si>
-    <t xml:space="preserve">Scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">limit_linear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">limit_log</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scenario for PKParameter, for Range plots comma separatedList is possible</t>
   </si>
   <si>
-    <t xml:space="preserve">used for comparsion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">corresponds to name (identifier) of model or PK parameter, comma seperated list is split to plots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Needed only  if ParameterId is PKParameter, comma separated List is split to facets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if filled parameter is displayed as range plot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mode how to creates the bins, needed if parameterId_Bin is given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">for “custom binning”  bin borders (soemthing like c(1,2,3)) otherwise number of bins. Needed if parameterId_Bin is given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scale of  x (histograms) or y (rangplots) axis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">limit used of linear scale, should be something like c(0,NA) to set lower limit to 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">limit used of log scale, should be something like c(0.1,NA) to set lower limit to 0.1</t>
+    <t xml:space="preserve">Model parameter id used to bin , displayed o x-axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mode how to creates the bins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for “custom binning”  bin borders (soemthing like c(1,2,3)) otherwise number of bins.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scale of  y axis</t>
   </si>
   <si>
     <t xml:space="preserve">SensitivityParameterSheet</t>
@@ -1085,7 +1083,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="I1:I2 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1133,10 +1131,300 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:XFD40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K18" activeCellId="1" sqref="I1:I2 K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="27" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="XFD1" s="1"/>
+    </row>
+    <row r="2" s="30" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="XFD2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M4" s="20"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M5" s="20"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="20"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M7" s="20"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M9" s="20"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M10" s="20"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M11" s="20"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" s="20"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="20"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" s="20"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="20"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="20"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M17" s="20"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="20"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" s="20"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M21" s="20"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M22" s="20"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M23" s="20"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M24" s="20"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M25" s="20"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M26" s="20"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M27" s="20"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M28" s="20"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M29" s="20"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M30" s="20"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M31" s="20"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M32" s="20"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M33" s="20"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M34" s="20"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M35" s="20"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M36" s="20"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M37" s="20"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M38" s="20"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M39" s="20"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M40" s="20"/>
+    </row>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J1:J2" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="I3:I1002 K3:L1002" type="list">
+      <formula1>Outputs!$A$3:$A$100</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P3:P1002" type="list">
+      <formula1>"fixed,free_y,free_x,free"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M4:M1002" type="list">
+      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="x12ac">
+          <x12ac:list>"linear, log",linear,log</x12ac:list>
+        </mc:Choice>
+        <mc:Fallback>
+          <formula1>"linear, log,linear,log"</formula1>
+        </mc:Fallback>
+      </mc:AlternateContent>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M3" type="list">
+      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="x12ac">
+          <x12ac:list>"linear, log",linear,log</x12ac:list>
+        </mc:Choice>
+        <mc:Fallback>
+          <formula1>"linear, log,linear,log"</formula1>
+        </mc:Fallback>
+      </mc:AlternateContent>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J3:J1002" type="list">
+      <formula1>"Equal Frequency Binning,Equal Width Binning,Custom Binning"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1165,31 +1453,37 @@
         <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>162</v>
+      <c r="I1" s="13" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="15"/>
       <c r="C2" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>165</v>
+      <c r="I2" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1217,7 +1511,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="I1:I2 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1314,7 +1608,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I1:I2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1386,7 +1680,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="I1:I2 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1527,7 +1821,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1873,7 +2167,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="I1:I2 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1964,7 +2258,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="I1:I2 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2230,7 +2524,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="N3" activeCellId="1" sqref="I1:I2 N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2446,7 +2740,11 @@
       <c r="K40" s="20"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N1:N2" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="H3:I1002" type="list">
       <formula1>Outputs!$A$3:$A$100</formula1>
       <formula2>0</formula2>
@@ -2462,12 +2760,12 @@
       </mc:AlternateContent>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N3:N1002" type="list">
-      <formula1>"fixed,free_y,free_x,free"</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="J3:J1002" type="list">
+      <formula1>DataGroups!$A$3:$A$100</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="J3:J1002" type="list">
-      <formula1>DataGroups!$A$3:$A$100</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N3:N1002" type="list">
+      <formula1>"free_y,free"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2488,8 +2786,8 @@
   </sheetPr>
   <dimension ref="A1:XFD40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="I1:I2 J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2499,10 +2797,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" s="27" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2516,7 +2815,7 @@
         <v>59</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>67</v>
@@ -2525,38 +2824,32 @@
         <v>69</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H1" s="31" t="s">
         <v>61</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>144</v>
+        <v>64</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="P1" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="XFA1" s="1"/>
+      <c r="XFB1" s="1"/>
+      <c r="XFC1" s="1"/>
       <c r="XFD1" s="1"/>
     </row>
     <row r="2" s="30" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2566,167 +2859,161 @@
         <v>123</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>92</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="P2" s="18" t="s">
         <v>95</v>
       </c>
+      <c r="XFA2" s="1"/>
+      <c r="XFB2" s="1"/>
+      <c r="XFC2" s="1"/>
       <c r="XFD2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M3" s="20"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M5" s="20"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M6" s="20"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M8" s="20"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M9" s="20"/>
+      <c r="J9" s="20"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M10" s="20"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M11" s="20"/>
+      <c r="J11" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M12" s="20"/>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M13" s="20"/>
+      <c r="J13" s="20"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M14" s="20"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M15" s="20"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M16" s="20"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M17" s="20"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M18" s="20"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M20" s="20"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M21" s="20"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M22" s="20"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M23" s="20"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M24" s="20"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M25" s="20"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M26" s="20"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M27" s="20"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M28" s="20"/>
+      <c r="J28" s="20"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M29" s="20"/>
+      <c r="J29" s="20"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M32" s="20"/>
+      <c r="J32" s="20"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M33" s="20"/>
+      <c r="J33" s="20"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M34" s="20"/>
+      <c r="J34" s="20"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M35" s="20"/>
+      <c r="J35" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M36" s="20"/>
+      <c r="J36" s="20"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M37" s="20"/>
+      <c r="J37" s="20"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M38" s="20"/>
+      <c r="J38" s="20"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M39" s="20"/>
+      <c r="J39" s="20"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M40" s="20"/>
+      <c r="J40" s="20"/>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P3:P1002" type="list">
+  <dataValidations count="4">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M3:M1002" type="list">
       <formula1>"fixed,free_y,free_x,free"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M4:M1002" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J4:J1002" type="list">
       <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
         <mc:Choice Requires="x12ac">
           <x12ac:list>"linear, log",linear,log</x12ac:list>
@@ -2737,11 +3024,11 @@
       </mc:AlternateContent>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="I3:I1002 K3:L1002" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="I3:I1002" type="list">
       <formula1>Outputs!$A$3:$A$100</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M3" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J3" type="list">
       <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
         <mc:Choice Requires="x12ac">
           <x12ac:list>"linear, log",linear,log</x12ac:list>
@@ -2750,14 +3037,6 @@
           <formula1>"linear, log,linear,log"</formula1>
         </mc:Fallback>
       </mc:AlternateContent>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J3:J1002" type="list">
-      <formula1>"Equal Frequency Binning,Equal Width Binning,Custom Binning"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J1:J2" type="none">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
build of tests an ddocumentation
</commit_message>
<xml_diff>
--- a/inst/templates/Plots.xlsx
+++ b/inst/templates/Plots.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" state="visible" r:id="rId3"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="168">
   <si>
     <t xml:space="preserve">Scenario</t>
   </si>
@@ -254,7 +254,10 @@
     <t xml:space="preserve">yScale</t>
   </si>
   <si>
-    <t xml:space="preserve">FacetType</t>
+    <t xml:space="preserve">SplitPlotsPerTimeRange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nFacetColumns</t>
   </si>
   <si>
     <t xml:space="preserve">FacetScale</t>
@@ -315,6 +318,12 @@
   </si>
   <si>
     <t xml:space="preserve">scale of y axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if true (1) for each time range a special plot is created, if false (0) time ranges are displayed different panels in one plot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of facet columns</t>
   </si>
   <si>
     <t xml:space="preserve">passed on to facet_wrap , scales</t>
@@ -694,7 +703,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -755,6 +764,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -771,6 +784,10 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -826,10 +843,6 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1083,7 +1096,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="I1:I2 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="T1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1134,7 +1147,7 @@
   <dimension ref="A1:XFD40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="1" sqref="I1:I2 K18"/>
+      <selection pane="topLeft" activeCell="K18" activeCellId="1" sqref="T1 K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1150,39 +1163,39 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="28" t="s">
         <v>67</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="H1" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="33" t="s">
         <v>61</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>64</v>
@@ -1191,188 +1204,188 @@
         <v>73</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+        <v>76</v>
+      </c>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
       <c r="XFD1" s="1"/>
     </row>
-    <row r="2" s="30" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="K2" s="18" t="s">
+    <row r="2" s="32" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L2" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" s="18" t="s">
+      <c r="E2" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="N2" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>95</v>
+      <c r="J2" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="XFD2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M3" s="20"/>
+      <c r="M3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M4" s="20"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M5" s="20"/>
+      <c r="M5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M6" s="20"/>
+      <c r="M6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M7" s="20"/>
+      <c r="M7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M8" s="20"/>
+      <c r="M8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M9" s="20"/>
+      <c r="M9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M10" s="20"/>
+      <c r="M10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M11" s="20"/>
+      <c r="M11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M12" s="20"/>
+      <c r="M12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M13" s="20"/>
+      <c r="M13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M14" s="20"/>
+      <c r="M14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M15" s="20"/>
+      <c r="M15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M16" s="20"/>
+      <c r="M16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M17" s="20"/>
+      <c r="M17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M18" s="20"/>
+      <c r="M18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M19" s="20"/>
+      <c r="M19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M20" s="20"/>
+      <c r="M20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M21" s="20"/>
+      <c r="M21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M22" s="20"/>
+      <c r="M22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M23" s="20"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M24" s="20"/>
+      <c r="M24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M25" s="20"/>
+      <c r="M25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M26" s="20"/>
+      <c r="M26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M27" s="20"/>
+      <c r="M27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M28" s="20"/>
+      <c r="M28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M29" s="20"/>
+      <c r="M29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M30" s="20"/>
+      <c r="M30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M31" s="20"/>
+      <c r="M31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M32" s="20"/>
+      <c r="M32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M33" s="20"/>
+      <c r="M33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M34" s="20"/>
+      <c r="M34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M35" s="20"/>
+      <c r="M35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M36" s="20"/>
+      <c r="M36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M37" s="20"/>
+      <c r="M37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M38" s="20"/>
+      <c r="M38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M39" s="20"/>
+      <c r="M39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M40" s="20"/>
+      <c r="M40" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="6">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="I3:I1002 K3:L1002" type="list">
+      <formula1>Outputs!$A$3:$A$100</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J1:J2" type="none">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="I3:I1002 K3:L1002" type="list">
-      <formula1>Outputs!$A$3:$A$100</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P3:P1002" type="list">
@@ -1423,8 +1436,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1:I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="T1 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1453,13 +1466,13 @@
         <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>64</v>
@@ -1467,23 +1480,23 @@
     </row>
     <row r="2" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16" t="s">
-        <v>162</v>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1511,7 +1524,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="I1:I2 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="T1 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1608,7 +1621,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I1:I2 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1680,7 +1693,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="I1:I2 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="T1 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1814,14 +1827,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC40"/>
+  <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1:I2"/>
+      <selection pane="bottomRight" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1831,7 +1844,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="9.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1889,28 +1902,28 @@
       <c r="R1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="12" t="s">
         <v>77</v>
       </c>
       <c r="W1" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Y1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="13" t="s">
         <v>81</v>
       </c>
       <c r="AA1" s="12" t="s">
@@ -1922,203 +1935,283 @@
       <c r="AC1" s="12" t="s">
         <v>84</v>
       </c>
+      <c r="AD1" s="12" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16" t="s">
-        <v>85</v>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2" s="17" t="s">
-        <v>90</v>
+      <c r="K2" s="18" t="s">
+        <v>91</v>
       </c>
       <c r="L2" s="3"/>
-      <c r="M2" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="N2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>92</v>
       </c>
+      <c r="N2" s="19" t="s">
+        <v>93</v>
+      </c>
       <c r="O2" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3" t="s">
+      <c r="R2" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="S2" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="T2" s="20" t="s">
         <v>97</v>
       </c>
+      <c r="U2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>99</v>
+      </c>
       <c r="W2" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="X2" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="Z2" s="16" t="s">
+      <c r="X2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AA2" s="16" t="s">
+      <c r="Y2" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="AB2" s="16" t="s">
+      <c r="Z2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AC2" s="16" t="s">
+      <c r="AA2" s="17" t="s">
         <v>104</v>
       </c>
+      <c r="AB2" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC2" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD2" s="17" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="R3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R4" s="20"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R5" s="20"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R6" s="20"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R7" s="20"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R8" s="20"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R9" s="20"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R10" s="20"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R11" s="20"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R12" s="20"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R13" s="20"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R14" s="20"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R15" s="20"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R16" s="20"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R17" s="20"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R18" s="20"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R19" s="20"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R20" s="20"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R21" s="20"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R22" s="20"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R23" s="20"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R24" s="20"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R25" s="20"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R26" s="20"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R27" s="20"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R28" s="20"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R29" s="20"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R30" s="20"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R31" s="20"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R32" s="20"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R33" s="20"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R34" s="20"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R35" s="20"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R36" s="20"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R37" s="20"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R38" s="20"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R39" s="20"/>
+      <c r="R39" s="22"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R40" s="20"/>
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
     </row>
   </sheetData>
-  <dataValidations count="7">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U3:U1002 X3:AB1002" type="list">
+  <dataValidations count="8">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V3:V1002 Y3:AC1002" type="list">
       <formula1>"1,0"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S3:S1002" type="list">
-      <formula1>"by order,by Individual,Senario vs Output,Scenario vs TimeRange"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J3:J1002" type="list">
@@ -2136,7 +2229,7 @@
       </mc:AlternateContent>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T3:T1002" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U3:U1002" type="list">
       <formula1>"fixed,free_y,free_x,free"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2146,6 +2239,14 @@
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="F3:F1002" type="list">
       <formula1>Outputs!$A$3:$A$100</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S1:T2 T3:T1002" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S3:S1002" type="list">
+      <formula1>"1,0"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2167,7 +2268,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="I1:I2 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="T1 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2179,39 +2280,39 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>108</v>
       </c>
+      <c r="B1" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>112</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0</v>
@@ -2219,24 +2320,24 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2258,7 +2359,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="I1:I2 H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="T1 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2276,29 +2377,29 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.29"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="28" t="s">
         <v>67</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="28" t="s">
         <v>61</v>
       </c>
       <c r="I1" s="13" t="s">
@@ -2308,177 +2409,177 @@
         <v>73</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>121</v>
+        <v>76</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>124</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" s="30" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="18" t="s">
+    </row>
+    <row r="2" s="32" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="I2" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" s="18" t="s">
+      <c r="E2" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>129</v>
+      <c r="N2" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J3" s="20"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J4" s="20"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J5" s="20"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="20"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J7" s="20"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J8" s="20"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J9" s="20"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J10" s="20"/>
+      <c r="J10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="20"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="20"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J13" s="20"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="20"/>
+      <c r="J14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="20"/>
+      <c r="J15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="20"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="20"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="20"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="20"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="20"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="20"/>
+      <c r="J21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="20"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="20"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="20"/>
+      <c r="J24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="20"/>
+      <c r="J25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="20"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="20"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="20"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="20"/>
+      <c r="J29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="20"/>
+      <c r="J30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="20"/>
+      <c r="J31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="20"/>
+      <c r="J32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="20"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="20"/>
+      <c r="J34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="20"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="20"/>
+      <c r="J36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="20"/>
+      <c r="J37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="20"/>
+      <c r="J38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="20"/>
+      <c r="J39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="20"/>
+      <c r="J40" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2524,7 +2625,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="1" sqref="I1:I2 N3"/>
+      <selection pane="topLeft" activeCell="N3" activeCellId="1" sqref="T1 N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2541,203 +2642,203 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="28" t="s">
         <v>67</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="28" t="s">
         <v>61</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="26" t="s">
-        <v>131</v>
+      <c r="J1" s="28" t="s">
+        <v>134</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" s="30" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" s="32" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="E2" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="I2" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="N2" s="18" t="s">
-        <v>95</v>
+      <c r="K2" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K3" s="20"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="20"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K5" s="20"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K6" s="20"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K7" s="20"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K8" s="20"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K9" s="20"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K10" s="20"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K11" s="20"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K12" s="20"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K13" s="20"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K14" s="20"/>
+      <c r="K14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K15" s="20"/>
+      <c r="K15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K16" s="20"/>
+      <c r="K16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K17" s="20"/>
+      <c r="K17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K18" s="20"/>
+      <c r="K18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K19" s="20"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K20" s="20"/>
+      <c r="K20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K21" s="20"/>
+      <c r="K21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K22" s="20"/>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K23" s="20"/>
+      <c r="K23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K24" s="20"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K25" s="20"/>
+      <c r="K25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K26" s="20"/>
+      <c r="K26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K27" s="20"/>
+      <c r="K27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K28" s="20"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K29" s="20"/>
+      <c r="K29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K30" s="20"/>
+      <c r="K30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K31" s="20"/>
+      <c r="K31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K32" s="20"/>
+      <c r="K32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K33" s="20"/>
+      <c r="K33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K34" s="20"/>
+      <c r="K34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K35" s="20"/>
+      <c r="K35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K36" s="20"/>
+      <c r="K36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K37" s="20"/>
+      <c r="K37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K38" s="20"/>
+      <c r="K38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K39" s="20"/>
+      <c r="K39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K40" s="20"/>
+      <c r="K40" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2787,7 +2888,7 @@
   <dimension ref="A1:XFD40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="I1:I2 J2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="T1 J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2804,89 +2905,89 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="28" t="s">
         <v>67</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="H1" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="33" t="s">
         <v>61</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>64</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
+        <v>76</v>
+      </c>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
       <c r="XFA1" s="1"/>
       <c r="XFB1" s="1"/>
       <c r="XFC1" s="1"/>
       <c r="XFD1" s="1"/>
     </row>
-    <row r="2" s="30" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="H2" s="18" t="s">
+    <row r="2" s="32" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="I2" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="F2" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="M2" s="18" t="s">
-        <v>95</v>
+      <c r="I2" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="XFA2" s="1"/>
       <c r="XFB2" s="1"/>
@@ -2894,118 +2995,118 @@
       <c r="XFD2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J3" s="20"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J4" s="20"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J5" s="20"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="20"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J7" s="20"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J8" s="20"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J9" s="20"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J10" s="20"/>
+      <c r="J10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="20"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="20"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J13" s="20"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="20"/>
+      <c r="J14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="20"/>
+      <c r="J15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="20"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="20"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="20"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="20"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="20"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="20"/>
+      <c r="J21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="20"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="20"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="20"/>
+      <c r="J24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="20"/>
+      <c r="J25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="20"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="20"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="20"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="20"/>
+      <c r="J29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="20"/>
+      <c r="J30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="20"/>
+      <c r="J31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="20"/>
+      <c r="J32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="20"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="20"/>
+      <c r="J34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="20"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="20"/>
+      <c r="J36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="20"/>
+      <c r="J37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="20"/>
+      <c r="J38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="20"/>
+      <c r="J39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="20"/>
+      <c r="J40" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="4">

</xml_diff>

<commit_message>
Update testss and documentation
</commit_message>
<xml_diff>
--- a/inst/templates/Plots.xlsx
+++ b/inst/templates/Plots.xlsx
@@ -1096,7 +1096,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="T1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1147,7 +1147,7 @@
   <dimension ref="A1:XFD40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="1" sqref="T1 K18"/>
+      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1380,12 +1380,12 @@
     </row>
   </sheetData>
   <dataValidations count="6">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J1:J2" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="I3:I1002 K3:L1002" type="list">
       <formula1>Outputs!$A$3:$A$100</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J1:J2" type="none">
-      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P3:P1002" type="list">
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="T1 I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1524,7 +1524,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="T1 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1621,7 +1621,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1693,7 +1693,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="T1 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1830,11 +1830,11 @@
   <dimension ref="A1:AD40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="bottomRight" activeCell="AD3" activeCellId="0" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2209,8 +2209,8 @@
       <c r="T40" s="22"/>
     </row>
   </sheetData>
-  <dataValidations count="8">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V3:V1002 Y3:AC1002" type="list">
+  <dataValidations count="12">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V3:V1002 Y3:Y1002 AA3:AC1002" type="list">
       <formula1>"1,0"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2241,12 +2241,28 @@
       <formula1>Outputs!$A$3:$A$100</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S1:T2 T3:T1002" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S1:T2 Z1:Z1002 T3:T1002" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S3:S1002" type="list">
       <formula1>"1,0"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D3:D1002" type="list">
+      <formula1>Scenarios!$A$3:$A$100</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D1:D2" type="none">
+      <formula1>Scenarios!$A$3:$A$100</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L3:L1002" type="list">
+      <formula1>Scenarios!$A$3:$A$100</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L1:L2" type="none">
+      <formula1>Scenarios!$A$3:$A$100</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2268,7 +2284,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="T1 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2359,7 +2375,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="T1 H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2625,7 +2641,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="1" sqref="T1 N3"/>
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2888,7 +2904,7 @@
   <dimension ref="A1:XFD40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="T1 J2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update Vignette for plot creation
</commit_message>
<xml_diff>
--- a/inst/templates/Plots.xlsx
+++ b/inst/templates/Plots.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" state="visible" r:id="rId3"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="163">
   <si>
     <t xml:space="preserve">Scenario</t>
   </si>
@@ -65,15 +65,6 @@
     <t xml:space="preserve">Reference</t>
   </si>
   <si>
-    <t xml:space="preserve">DataSection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Route</t>
-  </si>
-  <si>
     <t xml:space="preserve">DefaultScenario</t>
   </si>
   <si>
@@ -83,19 +74,13 @@
     <t xml:space="preserve">group identifier used in observed, typcially a study arm</t>
   </si>
   <si>
-    <t xml:space="preserve">study number of data</t>
+    <t xml:space="preserve">meta data, just for information</t>
   </si>
   <si>
     <t xml:space="preserve">name used in report </t>
   </si>
   <si>
     <t xml:space="preserve">reference used in figure footnotes in report for timeprofiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">used for substructure of electronic package</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meta data used for electronic package data</t>
   </si>
   <si>
     <t xml:space="preserve">used as suggestion for plots</t>
@@ -544,7 +529,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +583,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -703,7 +695,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -728,6 +720,10 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -788,11 +784,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -800,7 +796,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1163,220 +1159,220 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="27" t="s">
+    <row r="1" s="30" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="M1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="XFD1" s="1"/>
+    </row>
+    <row r="2" s="33" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="13" t="s">
+      <c r="J2" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K2" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L2" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="L1" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="XFD1" s="1"/>
-    </row>
-    <row r="2" s="32" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="E2" s="19" t="s">
+      <c r="N2" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="O2" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="P2" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="N2" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>98</v>
-      </c>
       <c r="XFD2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M3" s="22"/>
+      <c r="M3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M4" s="22"/>
+      <c r="M4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M5" s="22"/>
+      <c r="M5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M6" s="22"/>
+      <c r="M6" s="23"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M7" s="22"/>
+      <c r="M7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M8" s="22"/>
+      <c r="M8" s="23"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M9" s="22"/>
+      <c r="M9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M10" s="22"/>
+      <c r="M10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M11" s="22"/>
+      <c r="M11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M12" s="22"/>
+      <c r="M12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M13" s="22"/>
+      <c r="M13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M14" s="22"/>
+      <c r="M14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M15" s="22"/>
+      <c r="M15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M16" s="22"/>
+      <c r="M16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M17" s="22"/>
+      <c r="M17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M18" s="22"/>
+      <c r="M18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M19" s="22"/>
+      <c r="M19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M20" s="22"/>
+      <c r="M20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M21" s="22"/>
+      <c r="M21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M22" s="22"/>
+      <c r="M22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M23" s="22"/>
+      <c r="M23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M24" s="22"/>
+      <c r="M24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M25" s="22"/>
+      <c r="M25" s="23"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M26" s="22"/>
+      <c r="M26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M27" s="22"/>
+      <c r="M27" s="23"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M28" s="22"/>
+      <c r="M28" s="23"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M29" s="22"/>
+      <c r="M29" s="23"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M30" s="22"/>
+      <c r="M30" s="23"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M31" s="22"/>
+      <c r="M31" s="23"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M32" s="22"/>
+      <c r="M32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M33" s="22"/>
+      <c r="M33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M34" s="22"/>
+      <c r="M34" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M35" s="22"/>
+      <c r="M35" s="23"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M36" s="22"/>
+      <c r="M36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M37" s="22"/>
+      <c r="M37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M38" s="22"/>
+      <c r="M38" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M39" s="22"/>
+      <c r="M39" s="23"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M40" s="22"/>
+      <c r="M40" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="6">
@@ -1450,53 +1446,53 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>59</v>
+      <c r="A1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>64</v>
+        <v>159</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17" t="s">
-        <v>165</v>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
+        <v>160</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1523,7 +1519,7 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1531,10 +1527,8 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="23.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="29.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1559,48 +1553,35 @@
       <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+    </row>
+    <row r="2" s="7" customFormat="true" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" s="6" customFormat="true" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1634,44 +1615,44 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" s="8" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1704,111 +1685,111 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1829,7 +1810,7 @@
   </sheetPr>
   <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
@@ -1848,365 +1829,365 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>59</v>
+      <c r="A1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="K1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="N1" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="O1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="P1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="S1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="T1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="U1" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="V1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="W1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="X1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="Y1" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="Z1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="AA1" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="AD1" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="Z1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA1" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB1" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC1" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD1" s="12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17" t="s">
-        <v>86</v>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="N2" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="N2" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="18" t="s">
+      <c r="R2" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="X2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="Y2" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="AA2" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="AB2" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="AC2" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="AD2" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="Z2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AA2" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="AB2" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC2" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD2" s="17" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="22"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R21" s="22"/>
-      <c r="S21" s="22"/>
-      <c r="T21" s="22"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="22"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="22"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R25" s="22"/>
-      <c r="S25" s="22"/>
-      <c r="T25" s="22"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="22"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R29" s="22"/>
-      <c r="S29" s="22"/>
-      <c r="T29" s="22"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R30" s="22"/>
-      <c r="S30" s="22"/>
-      <c r="T30" s="22"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="23"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R31" s="22"/>
-      <c r="S31" s="22"/>
-      <c r="T31" s="22"/>
+      <c r="R31" s="23"/>
+      <c r="S31" s="23"/>
+      <c r="T31" s="23"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R32" s="22"/>
-      <c r="S32" s="22"/>
-      <c r="T32" s="22"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R33" s="22"/>
-      <c r="S33" s="22"/>
-      <c r="T33" s="22"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="23"/>
+      <c r="T33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R34" s="22"/>
-      <c r="S34" s="22"/>
-      <c r="T34" s="22"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23"/>
+      <c r="T34" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R35" s="22"/>
-      <c r="S35" s="22"/>
-      <c r="T35" s="22"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="23"/>
+      <c r="T35" s="23"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R36" s="22"/>
-      <c r="S36" s="22"/>
-      <c r="T36" s="22"/>
+      <c r="R36" s="23"/>
+      <c r="S36" s="23"/>
+      <c r="T36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R37" s="22"/>
-      <c r="S37" s="22"/>
-      <c r="T37" s="22"/>
+      <c r="R37" s="23"/>
+      <c r="S37" s="23"/>
+      <c r="T37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R38" s="22"/>
-      <c r="S38" s="22"/>
-      <c r="T38" s="22"/>
+      <c r="R38" s="23"/>
+      <c r="S38" s="23"/>
+      <c r="T38" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R39" s="22"/>
-      <c r="S39" s="22"/>
-      <c r="T39" s="22"/>
+      <c r="R39" s="23"/>
+      <c r="S39" s="23"/>
+      <c r="T39" s="23"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R40" s="22"/>
-      <c r="S40" s="22"/>
-      <c r="T40" s="22"/>
+      <c r="R40" s="23"/>
+      <c r="S40" s="23"/>
+      <c r="T40" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="12">
@@ -2290,70 +2271,70 @@
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C2" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D2" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="23" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
+      <c r="C3" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>119</v>
+      <c r="A4" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2393,209 +2374,209 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.29"/>
   </cols>
   <sheetData>
-    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="27" t="s">
+    <row r="1" s="30" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="J1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" s="33" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="27" t="s">
+      <c r="F2" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="H2" s="20" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" s="32" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
+      <c r="I2" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="O2" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="N2" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>132</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J3" s="22"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J4" s="22"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J5" s="22"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="22"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J7" s="22"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J8" s="22"/>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J9" s="22"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J10" s="22"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="22"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="22"/>
+      <c r="J12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J13" s="22"/>
+      <c r="J13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="22"/>
+      <c r="J14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="22"/>
+      <c r="J15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="22"/>
+      <c r="J16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="22"/>
+      <c r="J17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="22"/>
+      <c r="J18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="22"/>
+      <c r="J19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="22"/>
+      <c r="J20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="22"/>
+      <c r="J21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="22"/>
+      <c r="J22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="22"/>
+      <c r="J23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="22"/>
+      <c r="J24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="22"/>
+      <c r="J25" s="23"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="22"/>
+      <c r="J26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="22"/>
+      <c r="J27" s="23"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="22"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="22"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="22"/>
+      <c r="J30" s="23"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="22"/>
+      <c r="J31" s="23"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="22"/>
+      <c r="J32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="22"/>
+      <c r="J33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="22"/>
+      <c r="J34" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="22"/>
+      <c r="J35" s="23"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="22"/>
+      <c r="J36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="22"/>
+      <c r="J37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="22"/>
+      <c r="J38" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="22"/>
+      <c r="J39" s="23"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="22"/>
+      <c r="J40" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2658,203 +2639,203 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="27" t="s">
+    <row r="1" s="30" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="J1" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" s="33" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="E2" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="28" t="s">
+      <c r="G2" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="H2" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="I2" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="K2" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" s="32" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="19" t="s">
+      <c r="L2" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="19" t="s">
+      <c r="M2" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="N2" s="19" t="s">
-        <v>98</v>
+      <c r="N2" s="20" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K3" s="22"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="22"/>
+      <c r="K4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K5" s="22"/>
+      <c r="K5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K6" s="22"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K7" s="22"/>
+      <c r="K7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K8" s="22"/>
+      <c r="K8" s="23"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K9" s="22"/>
+      <c r="K9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K10" s="22"/>
+      <c r="K10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K11" s="22"/>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K12" s="22"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K13" s="22"/>
+      <c r="K13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K14" s="22"/>
+      <c r="K14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K15" s="22"/>
+      <c r="K15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K16" s="22"/>
+      <c r="K16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K17" s="22"/>
+      <c r="K17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K18" s="22"/>
+      <c r="K18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K19" s="22"/>
+      <c r="K19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K20" s="22"/>
+      <c r="K20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K21" s="22"/>
+      <c r="K21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K22" s="22"/>
+      <c r="K22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K23" s="22"/>
+      <c r="K23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K24" s="22"/>
+      <c r="K24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K25" s="22"/>
+      <c r="K25" s="23"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K26" s="22"/>
+      <c r="K26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K27" s="22"/>
+      <c r="K27" s="23"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K28" s="22"/>
+      <c r="K28" s="23"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K29" s="22"/>
+      <c r="K29" s="23"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K30" s="22"/>
+      <c r="K30" s="23"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K31" s="22"/>
+      <c r="K31" s="23"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K32" s="22"/>
+      <c r="K32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K33" s="22"/>
+      <c r="K33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K34" s="22"/>
+      <c r="K34" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K35" s="22"/>
+      <c r="K35" s="23"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K36" s="22"/>
+      <c r="K36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K37" s="22"/>
+      <c r="K37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K38" s="22"/>
+      <c r="K38" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K39" s="22"/>
+      <c r="K39" s="23"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K40" s="22"/>
+      <c r="K40" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2921,89 +2902,89 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="27" t="s">
+    <row r="1" s="30" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
+      <c r="J1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
       <c r="XFA1" s="1"/>
       <c r="XFB1" s="1"/>
       <c r="XFC1" s="1"/>
       <c r="XFD1" s="1"/>
     </row>
-    <row r="2" s="32" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="20" t="s">
+    <row r="2" s="33" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="L2" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="M2" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>98</v>
       </c>
       <c r="XFA2" s="1"/>
       <c r="XFB2" s="1"/>
@@ -3011,118 +2992,118 @@
       <c r="XFD2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J3" s="22"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J4" s="22"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J5" s="22"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="22"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J7" s="22"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J8" s="22"/>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J9" s="22"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J10" s="22"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="22"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="22"/>
+      <c r="J12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J13" s="22"/>
+      <c r="J13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="22"/>
+      <c r="J14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="22"/>
+      <c r="J15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="22"/>
+      <c r="J16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="22"/>
+      <c r="J17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="22"/>
+      <c r="J18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="22"/>
+      <c r="J19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="22"/>
+      <c r="J20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="22"/>
+      <c r="J21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="22"/>
+      <c r="J22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="22"/>
+      <c r="J23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="22"/>
+      <c r="J24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="22"/>
+      <c r="J25" s="23"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="22"/>
+      <c r="J26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="22"/>
+      <c r="J27" s="23"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="22"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="22"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="22"/>
+      <c r="J30" s="23"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="22"/>
+      <c r="J31" s="23"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="22"/>
+      <c r="J32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="22"/>
+      <c r="J33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="22"/>
+      <c r="J34" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="22"/>
+      <c r="J35" s="23"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="22"/>
+      <c r="J36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="22"/>
+      <c r="J37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="22"/>
+      <c r="J38" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="22"/>
+      <c r="J39" s="23"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="22"/>
+      <c r="J40" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="4">

</xml_diff>

<commit_message>
add testcase for timeprofile without data
</commit_message>
<xml_diff>
--- a/inst/templates/Plots.xlsx
+++ b/inst/templates/Plots.xlsx
@@ -529,7 +529,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,13 +583,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -695,7 +688,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -720,16 +713,12 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -784,11 +773,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -796,7 +785,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1159,220 +1148,220 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="30" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
       <c r="XFD1" s="1"/>
     </row>
-    <row r="2" s="33" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32" t="s">
+    <row r="2" s="32" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="O2" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="P2" s="19" t="s">
         <v>93</v>
       </c>
       <c r="XFD2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M3" s="23"/>
+      <c r="M3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M4" s="23"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M5" s="23"/>
+      <c r="M5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M6" s="23"/>
+      <c r="M6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M7" s="23"/>
+      <c r="M7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M8" s="23"/>
+      <c r="M8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M9" s="23"/>
+      <c r="M9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M10" s="23"/>
+      <c r="M10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M11" s="23"/>
+      <c r="M11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M12" s="23"/>
+      <c r="M12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M13" s="23"/>
+      <c r="M13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M14" s="23"/>
+      <c r="M14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M15" s="23"/>
+      <c r="M15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M16" s="23"/>
+      <c r="M16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M17" s="23"/>
+      <c r="M17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M18" s="23"/>
+      <c r="M18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M19" s="23"/>
+      <c r="M19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M20" s="23"/>
+      <c r="M20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M21" s="23"/>
+      <c r="M21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M22" s="23"/>
+      <c r="M22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M23" s="23"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M24" s="23"/>
+      <c r="M24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M25" s="23"/>
+      <c r="M25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M26" s="23"/>
+      <c r="M26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M27" s="23"/>
+      <c r="M27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M28" s="23"/>
+      <c r="M28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M29" s="23"/>
+      <c r="M29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M30" s="23"/>
+      <c r="M30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M31" s="23"/>
+      <c r="M31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M32" s="23"/>
+      <c r="M32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M33" s="23"/>
+      <c r="M33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M34" s="23"/>
+      <c r="M34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M35" s="23"/>
+      <c r="M35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M36" s="23"/>
+      <c r="M36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M37" s="23"/>
+      <c r="M37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M38" s="23"/>
+      <c r="M38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M39" s="23"/>
+      <c r="M39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M40" s="23"/>
+      <c r="M40" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="6">
@@ -1446,13 +1435,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1470,14 +1459,14 @@
       <c r="H1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="17" t="s">
         <v>160</v>
       </c>
       <c r="D2" s="3"/>
@@ -1520,7 +1509,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1528,7 +1517,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="23.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="29.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,14 +1543,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" s="7" customFormat="true" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="6" customFormat="true" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -1576,12 +1565,12 @@
       <c r="G2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8"/>
+      <c r="A3" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1615,7 +1604,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -1635,7 +1624,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="8" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -1788,7 +1777,7 @@
       <c r="C8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1829,13 +1818,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1853,22 +1842,22 @@
       <c r="H1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>61</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>64</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -1880,50 +1869,50 @@
       <c r="Q1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="X1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Y1" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AA1" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AB1" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AC1" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AD1" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="17" t="s">
         <v>81</v>
       </c>
       <c r="D2" s="3"/>
@@ -1941,14 +1930,14 @@
         <v>85</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>86</v>
       </c>
       <c r="L2" s="3"/>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="19" t="s">
         <v>88</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -1956,19 +1945,19 @@
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="19" t="s">
+      <c r="R2" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="S2" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="21" t="s">
+      <c r="T2" s="20" t="s">
         <v>92</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="V2" s="18" t="s">
+      <c r="V2" s="17" t="s">
         <v>94</v>
       </c>
       <c r="W2" s="3" t="s">
@@ -1977,217 +1966,217 @@
       <c r="X2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="Y2" s="18" t="s">
+      <c r="Y2" s="17" t="s">
         <v>97</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="AA2" s="18" t="s">
+      <c r="AA2" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="AB2" s="18" t="s">
+      <c r="AB2" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="AC2" s="18" t="s">
+      <c r="AC2" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="AD2" s="18" t="s">
+      <c r="AD2" s="17" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="23"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="23"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="23"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="23"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-      <c r="T31" s="23"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R33" s="23"/>
-      <c r="S33" s="23"/>
-      <c r="T33" s="23"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R34" s="23"/>
-      <c r="S34" s="23"/>
-      <c r="T34" s="23"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R35" s="23"/>
-      <c r="S35" s="23"/>
-      <c r="T35" s="23"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R36" s="23"/>
-      <c r="S36" s="23"/>
-      <c r="T36" s="23"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R37" s="23"/>
-      <c r="S37" s="23"/>
-      <c r="T37" s="23"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R38" s="23"/>
-      <c r="S38" s="23"/>
-      <c r="T38" s="23"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R39" s="23"/>
-      <c r="S39" s="23"/>
-      <c r="T39" s="23"/>
+      <c r="R39" s="22"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R40" s="23"/>
-      <c r="S40" s="23"/>
-      <c r="T40" s="23"/>
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="12">
@@ -2271,41 +2260,41 @@
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>111</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2316,10 +2305,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>114</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2327,10 +2316,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>116</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2374,209 +2363,209 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.29"/>
   </cols>
   <sheetData>
-    <row r="1" s="30" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" s="33" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32" t="s">
+    <row r="2" s="32" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="O2" s="19" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J3" s="23"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J4" s="23"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J5" s="23"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="23"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J7" s="23"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J8" s="23"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J9" s="23"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J10" s="23"/>
+      <c r="J10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="23"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="23"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J13" s="23"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="23"/>
+      <c r="J14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="23"/>
+      <c r="J15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="23"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="23"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="23"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="23"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="23"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="23"/>
+      <c r="J21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="23"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="23"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="23"/>
+      <c r="J24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="23"/>
+      <c r="J25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="23"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="23"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="23"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="23"/>
+      <c r="J29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="23"/>
+      <c r="J30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="23"/>
+      <c r="J31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="23"/>
+      <c r="J32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="23"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="23"/>
+      <c r="J34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="23"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="23"/>
+      <c r="J36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="23"/>
+      <c r="J37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="23"/>
+      <c r="J38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="23"/>
+      <c r="J39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="23"/>
+      <c r="J40" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2639,203 +2628,203 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="30" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" s="33" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32" t="s">
+    <row r="2" s="32" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="19" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K3" s="23"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="23"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K5" s="23"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K6" s="23"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K7" s="23"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K8" s="23"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K9" s="23"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K10" s="23"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K11" s="23"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K12" s="23"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K13" s="23"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K14" s="23"/>
+      <c r="K14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K15" s="23"/>
+      <c r="K15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K16" s="23"/>
+      <c r="K16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K17" s="23"/>
+      <c r="K17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K18" s="23"/>
+      <c r="K18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K19" s="23"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K20" s="23"/>
+      <c r="K20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K21" s="23"/>
+      <c r="K21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K22" s="23"/>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K23" s="23"/>
+      <c r="K23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K24" s="23"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K25" s="23"/>
+      <c r="K25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K26" s="23"/>
+      <c r="K26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K27" s="23"/>
+      <c r="K27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K28" s="23"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K29" s="23"/>
+      <c r="K29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K30" s="23"/>
+      <c r="K30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K31" s="23"/>
+      <c r="K31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K32" s="23"/>
+      <c r="K32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K33" s="23"/>
+      <c r="K33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K34" s="23"/>
+      <c r="K34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K35" s="23"/>
+      <c r="K35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K36" s="23"/>
+      <c r="K36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K37" s="23"/>
+      <c r="K37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K38" s="23"/>
+      <c r="K38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K39" s="23"/>
+      <c r="K39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K40" s="23"/>
+      <c r="K40" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2902,88 +2891,88 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="30" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+    <row r="1" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
       <c r="XFA1" s="1"/>
       <c r="XFB1" s="1"/>
       <c r="XFC1" s="1"/>
       <c r="XFD1" s="1"/>
     </row>
-    <row r="2" s="33" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32" t="s">
+    <row r="2" s="32" customFormat="true" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="19" t="s">
         <v>93</v>
       </c>
       <c r="XFA2" s="1"/>
@@ -2992,121 +2981,125 @@
       <c r="XFD2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J3" s="23"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J4" s="23"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J5" s="23"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="23"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J7" s="23"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J8" s="23"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J9" s="23"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J10" s="23"/>
+      <c r="J10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="23"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="23"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J13" s="23"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="23"/>
+      <c r="J14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="23"/>
+      <c r="J15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="23"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="23"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="23"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="23"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="23"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="23"/>
+      <c r="J21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="23"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="23"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="23"/>
+      <c r="J24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="23"/>
+      <c r="J25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="23"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="23"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="23"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="23"/>
+      <c r="J29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="23"/>
+      <c r="J30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="23"/>
+      <c r="J31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="23"/>
+      <c r="J32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="23"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="23"/>
+      <c r="J34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="23"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="23"/>
+      <c r="J36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="23"/>
+      <c r="J37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="23"/>
+      <c r="J38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="23"/>
+      <c r="J39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="23"/>
+      <c r="J40" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="4">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="I3:I1002" type="list">
+      <formula1>Outputs!$A$3:$A$100</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M3:M1002" type="list">
       <formula1>"fixed,free_y,free_x,free"</formula1>
       <formula2>0</formula2>
@@ -3120,10 +3113,6 @@
           <formula1>"linear, log,linear,log"</formula1>
         </mc:Fallback>
       </mc:AlternateContent>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="I3:I1002" type="list">
-      <formula1>Outputs!$A$3:$A$100</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J3" type="list">

</xml_diff>